<commit_message>
se crea el exel y se crea la opcion 2 para que el exel funcione como base local y se agregue pokemones si no los tiene
</commit_message>
<xml_diff>
--- a/pokemones.xlsx
+++ b/pokemones.xlsx
@@ -1,98 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\PROYECTOS CON PYTHON\poke_api\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A9E022-2574-4DF2-A4EE-722410E5E69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>TIPOS</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>------------------------------------------------</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                    L </t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -102,32 +56,89 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -206,6 +217,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -240,6 +252,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -263,7 +276,6 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
@@ -274,31 +286,31 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
@@ -320,7 +332,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -378,7 +390,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -391,13 +403,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -415,75 +426,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="13.5546875" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="2" max="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>NOMBRE</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>TIPO</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="n">
+        <v>94</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>gengar</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ghost, poison</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="18.75" customHeight="1">
+      <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>2</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>bulbasaur</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>grass, poison</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="18.75" customHeight="1">
+      <c r="A4" t="n">
+        <v>143</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>snorlax</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>voltorb</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>electric</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>101</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>electrode</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>electric</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>300</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>skitty</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>48</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>venonat</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>bug, poison</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>gholdengo</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>steel, ghost</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1020</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>gouging-fire</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>fire, dragon</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios que olvide subir, el programa hace peticiones get a la api usando la libreria request y hace un guardado en local en un archivo excel
</commit_message>
<xml_diff>
--- a/pokemones.xlsx
+++ b/pokemones.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
@@ -595,6 +595,21 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>25</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>pikachu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>electric</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>